<commit_message>
data reorganisation + daily entry
</commit_message>
<xml_diff>
--- a/Raw_SRB_data/Crizotinib_only/Crizotinib_SRB_data.xlsx
+++ b/Raw_SRB_data/Crizotinib_only/Crizotinib_SRB_data.xlsx
@@ -3300,49 +3300,350 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F10" s="2"/>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="B7">
+        <v>3.9E-2</v>
+      </c>
+      <c r="C7">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D7">
+        <v>0.04</v>
+      </c>
+      <c r="E7">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="F7">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G7">
+        <v>0.04</v>
+      </c>
+      <c r="H7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.04</v>
+      </c>
+      <c r="J7">
+        <v>0.04</v>
+      </c>
+      <c r="K7">
+        <v>3.9E-2</v>
+      </c>
+      <c r="L7">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.05</v>
+      </c>
+      <c r="B8">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C8">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D8">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E8">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="F8">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="G8">
+        <v>4.7E-2</v>
+      </c>
+      <c r="H8">
+        <v>4.7E-2</v>
+      </c>
+      <c r="I8">
+        <v>4.7E-2</v>
+      </c>
+      <c r="J8">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="K8">
+        <v>4.7E-2</v>
+      </c>
+      <c r="L8">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="B9">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="C9">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D9">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E9">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F9">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="G9">
+        <v>4.7E-2</v>
+      </c>
+      <c r="H9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="I9">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="J9">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="K9">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="L9">
+        <v>7.1999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.04</v>
+      </c>
+      <c r="B10">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C10">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D10">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E10">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="G10">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="H10">
+        <v>4.7E-2</v>
+      </c>
+      <c r="I10">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="J10">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="K10">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="L10">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.04</v>
+      </c>
+      <c r="B11">
+        <v>0.05</v>
+      </c>
+      <c r="C11">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D11">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E11">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F11">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="G11">
+        <v>0.06</v>
+      </c>
+      <c r="H11">
+        <v>0.06</v>
+      </c>
+      <c r="I11">
+        <v>6.2E-2</v>
+      </c>
+      <c r="J11">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="K11">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="L11">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3.9E-2</v>
+      </c>
+      <c r="B12">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="C12">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="D12">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="E12">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="F12">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G12">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="H12">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="I12">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="J12">
+        <v>0.06</v>
+      </c>
+      <c r="K12">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="L12">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3.9E-2</v>
+      </c>
+      <c r="B13">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C13">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D13">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E13">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G13">
+        <v>4.7E-2</v>
+      </c>
+      <c r="H13">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="I13">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="J13">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="K13">
+        <v>6.2E-2</v>
+      </c>
+      <c r="L13">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.04</v>
+      </c>
+      <c r="B14">
+        <v>0.04</v>
+      </c>
+      <c r="C14">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D14">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="E14">
+        <v>0.04</v>
+      </c>
+      <c r="F14">
+        <v>3.9E-2</v>
+      </c>
+      <c r="G14">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="H14">
+        <v>0.04</v>
+      </c>
+      <c r="I14">
+        <v>0.04</v>
+      </c>
+      <c r="J14">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="K14">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="L14">
+        <v>3.9E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating daily entry + obj summaries
</commit_message>
<xml_diff>
--- a/Raw_SRB_data/Crizotinib_only/Crizotinib_SRB_data.xlsx
+++ b/Raw_SRB_data/Crizotinib_only/Crizotinib_SRB_data.xlsx
@@ -3300,10 +3300,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:L14"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3383,34 +3383,34 @@
       <c r="A8">
         <v>0.05</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="7">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="7">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="7">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="7">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="7">
         <v>4.7E-2</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="7">
         <v>4.7E-2</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="7">
         <v>4.7E-2</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="7">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="7">
         <v>4.7E-2</v>
       </c>
       <c r="L8">
@@ -3421,34 +3421,34 @@
       <c r="A9">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="7">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="7">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="7">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="7">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="7">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="7">
         <v>4.7E-2</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="7">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="7">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="7">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="L9">
@@ -3459,34 +3459,34 @@
       <c r="A10">
         <v>0.04</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="7">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="7">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="7">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="7">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="7">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="7">
         <v>4.7E-2</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="7">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="7">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="7">
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="L10">
@@ -3643,6 +3643,137 @@
       </c>
       <c r="L14">
         <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>AVERAGE(B8:B10)</f>
+        <v>4.2333333333333334E-2</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:K18" si="0">AVERAGE(C8:C10)</f>
+        <v>4.4333333333333336E-2</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>4.5333333333333337E-2</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>4.4666666666666667E-2</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>4.2333333333333334E-2</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>4.766666666666667E-2</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>4.7333333333333338E-2</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>4.6666666666666669E-2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>4.8333333333333339E-2</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>4.8999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>4.2333333333333334E-2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>4.4333333333333336E-2</v>
+      </c>
+      <c r="C19" s="1">
+        <f>B19/0.0433*100</f>
+        <v>102.38645111624326</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>4.5333333333333337E-2</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" ref="C20:C27" si="1">B20/0.0433*100</f>
+        <v>104.69591993841418</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>4.4666666666666667E-2</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="1"/>
+        <v>103.15627405696691</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>4.2333333333333334E-2</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="1"/>
+        <v>97.767513471901466</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>4.766666666666667E-2</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="1"/>
+        <v>110.08468052347962</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>4.7333333333333338E-2</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="1"/>
+        <v>109.31485758275599</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>4.6666666666666669E-2</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="1"/>
+        <v>107.77521170130871</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>4.8333333333333339E-2</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="1"/>
+        <v>111.62432640492688</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>4.8999999999999995E-2</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="1"/>
+        <v>113.16397228637413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding raw data + fixing analysis
</commit_message>
<xml_diff>
--- a/Raw_SRB_data/Crizotinib_only/Crizotinib_SRB_data.xlsx
+++ b/Raw_SRB_data/Crizotinib_only/Crizotinib_SRB_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="C1" sheetId="6" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="C3" sheetId="4" r:id="rId3"/>
     <sheet name="C4" sheetId="3" r:id="rId4"/>
     <sheet name="C5" sheetId="1" r:id="rId5"/>
+    <sheet name="C6" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Crizotinib</t>
   </si>
@@ -97,6 +98,15 @@
   </si>
   <si>
     <t>Passage #9</t>
+  </si>
+  <si>
+    <t>Replicate # 6</t>
+  </si>
+  <si>
+    <t>Passage #10</t>
+  </si>
+  <si>
+    <t>Day  1 date: 25/7/19</t>
   </si>
 </sst>
 </file>
@@ -490,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54:C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,7 +1311,7 @@
         <v>0.80800000000000005</v>
       </c>
       <c r="C55" s="10">
-        <f>B55/0.8648*C54</f>
+        <f>B55/0.8648*100</f>
         <v>93.432007400555051</v>
       </c>
     </row>
@@ -1310,8 +1320,8 @@
         <v>0.75919999999999999</v>
       </c>
       <c r="C56" s="10">
-        <f t="shared" ref="C56:C63" si="1">B56/0.8648*C55</f>
-        <v>82.023103629164424</v>
+        <f t="shared" ref="C56:C63" si="1">B56/0.8648*100</f>
+        <v>87.789084181313598</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1320,7 +1330,7 @@
       </c>
       <c r="C57" s="10">
         <f t="shared" si="1"/>
-        <v>53.322605065120534</v>
+        <v>65.009250693802031</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1329,7 +1339,7 @@
       </c>
       <c r="C58" s="10">
         <f t="shared" si="1"/>
-        <v>9.1255152054091582</v>
+        <v>17.113783533765034</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1338,7 +1348,7 @@
       </c>
       <c r="C59" s="10">
         <f t="shared" si="1"/>
-        <v>7.6038925266163737</v>
+        <v>83.325624421831648</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1347,7 +1357,7 @@
       </c>
       <c r="C60" s="10">
         <f t="shared" si="1"/>
-        <v>1.1562348141189329</v>
+        <v>15.205827937095281</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1356,7 +1366,7 @@
       </c>
       <c r="C61" s="10">
         <f t="shared" si="1"/>
-        <v>0.15188283404707537</v>
+        <v>13.135985198889916</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1365,7 +1375,7 @@
       </c>
       <c r="C62" s="10">
         <f t="shared" si="1"/>
-        <v>1.6790008019080021E-2</v>
+        <v>11.054579093432006</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1374,7 +1384,7 @@
       </c>
       <c r="C63" s="10">
         <f t="shared" si="1"/>
-        <v>1.5881390563838407E-3</v>
+        <v>9.4588344125809414</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
@@ -1393,7 +1403,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C26" sqref="C26:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,7 +1960,7 @@
         <v>0.24479999999999999</v>
       </c>
       <c r="C27" s="1">
-        <f>B27/0.3042*C26</f>
+        <f>B27/0.3042*100</f>
         <v>80.473372781065081</v>
       </c>
     </row>
@@ -1959,8 +1969,8 @@
         <v>0.20519999999999999</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" ref="C28:C35" si="1">B28/0.3042*C27</f>
-        <v>54.283813591961049</v>
+        <f t="shared" ref="C28:C35" si="1">B28/0.3042*100</f>
+        <v>67.455621301775139</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
@@ -1969,7 +1979,7 @@
       </c>
       <c r="C29" s="1">
         <f t="shared" si="1"/>
-        <v>29.586641333159569</v>
+        <v>54.503616042077574</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
@@ -1978,7 +1988,7 @@
       </c>
       <c r="C30" s="1">
         <f t="shared" si="1"/>
-        <v>12.390986541237769</v>
+        <v>41.880341880341881</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -1987,7 +1997,7 @@
       </c>
       <c r="C31" s="1">
         <f t="shared" si="1"/>
-        <v>2.7291127490563127</v>
+        <v>22.024983563445097</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
@@ -1996,7 +2006,7 @@
       </c>
       <c r="C32" s="1">
         <f t="shared" si="1"/>
-        <v>0.50598934597888234</v>
+        <v>18.540433925049303</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -2005,7 +2015,7 @@
       </c>
       <c r="C33" s="1">
         <f t="shared" si="1"/>
-        <v>0.1011313354224722</v>
+        <v>19.986850756081523</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
@@ -2014,7 +2024,7 @@
       </c>
       <c r="C34" s="1">
         <f t="shared" si="1"/>
-        <v>1.9880518929203932E-2</v>
+        <v>19.658119658119656</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
@@ -2023,7 +2033,7 @@
       </c>
       <c r="C35" s="1">
         <f t="shared" si="1"/>
-        <v>3.1369655115114688E-3</v>
+        <v>15.779092702169626</v>
       </c>
     </row>
   </sheetData>
@@ -2036,8 +2046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2594,7 +2604,7 @@
         <v>0.33300000000000002</v>
       </c>
       <c r="C25" s="11">
-        <f>B25/0.3522*C24</f>
+        <f>B25/0.3522*100</f>
         <v>94.54855195911415</v>
       </c>
     </row>
@@ -2603,8 +2613,8 @@
         <v>0.3196</v>
       </c>
       <c r="C26" s="11">
-        <f t="shared" ref="C26:C33" si="1">B26/0.3522*C25</f>
-        <v>85.79703919969586</v>
+        <f t="shared" ref="C26:C33" si="1">B26/0.3522*100</f>
+        <v>90.743895513912548</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -2613,7 +2623,7 @@
       </c>
       <c r="C27" s="11">
         <f t="shared" si="1"/>
-        <v>69.13458184234436</v>
+        <v>80.579216354344112</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -2622,7 +2632,7 @@
       </c>
       <c r="C28" s="11">
         <f t="shared" si="1"/>
-        <v>40.47572622342819</v>
+        <v>58.546280522430436</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
@@ -2631,7 +2641,7 @@
       </c>
       <c r="C29" s="11">
         <f t="shared" si="1"/>
-        <v>9.768417742735366</v>
+        <v>24.134014764338442</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
@@ -2640,7 +2650,7 @@
       </c>
       <c r="C30" s="11">
         <f t="shared" si="1"/>
-        <v>1.8638207618166287</v>
+        <v>19.080068143100512</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -2649,7 +2659,7 @@
       </c>
       <c r="C31" s="11">
         <f t="shared" si="1"/>
-        <v>0.33868406801892176</v>
+        <v>18.171493469619534</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
@@ -2658,7 +2668,7 @@
       </c>
       <c r="C32" s="11">
         <f t="shared" si="1"/>
-        <v>6.4044176405622349E-2</v>
+        <v>18.909710391822827</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -2667,7 +2677,7 @@
       </c>
       <c r="C33" s="11">
         <f t="shared" si="1"/>
-        <v>9.9648519790690084E-3</v>
+        <v>15.559341283361727</v>
       </c>
     </row>
   </sheetData>
@@ -2681,7 +2691,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D20" sqref="D20:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3125,7 +3135,7 @@
         <v>1.0973333333333335</v>
       </c>
       <c r="D21" s="1">
-        <f>(C21/1.125333*D20)</f>
+        <f>(C21/1.125333*100)</f>
         <v>97.511877225082131</v>
       </c>
       <c r="F21" s="2"/>
@@ -3139,8 +3149,8 @@
         <v>1.0443333333333333</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" ref="D22:D29" si="1">(C22/1.125333*D21)</f>
-        <v>90.493128506904867</v>
+        <f t="shared" ref="D22:D29" si="1">(C22/1.125333*100)</f>
+        <v>92.802160190213328</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -3154,7 +3164,7 @@
       </c>
       <c r="D23" s="1">
         <f t="shared" si="1"/>
-        <v>70.925618766258609</v>
+        <v>78.376800467061756</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -3168,7 +3178,7 @@
       </c>
       <c r="D24" s="1">
         <f t="shared" si="1"/>
-        <v>43.025980527037369</v>
+        <v>60.663525078058377</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -3182,7 +3192,7 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" si="1"/>
-        <v>10.985902310488305</v>
+        <v>25.533182918596829</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -3196,7 +3206,7 @@
       </c>
       <c r="D26" s="1">
         <f t="shared" si="1"/>
-        <v>1.6823794955278282</v>
+        <v>15.313985578787195</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -3210,7 +3220,7 @@
       </c>
       <c r="D27" s="1">
         <f t="shared" si="1"/>
-        <v>0.21827086413271712</v>
+        <v>12.973937492280067</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -3224,7 +3234,7 @@
       </c>
       <c r="D28" s="1">
         <f t="shared" si="1"/>
-        <v>2.0107304162493837E-2</v>
+        <v>9.2120880367559366</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -3238,7 +3248,7 @@
       </c>
       <c r="D29" s="1">
         <f t="shared" si="1"/>
-        <v>1.5187689811033502E-3</v>
+        <v>7.5533197729027783</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -3302,8 +3312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3651,7 +3661,7 @@
         <v>4.2333333333333334E-2</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:K18" si="0">AVERAGE(C8:C10)</f>
+        <f t="shared" ref="C16:K16" si="0">AVERAGE(C8:C10)</f>
         <v>4.4333333333333336E-2</v>
       </c>
       <c r="D16">
@@ -3780,4 +3790,487 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="B7">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="C7">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="D7">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="E7">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.09</v>
+      </c>
+      <c r="G7">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="H7">
+        <v>7.8E-2</v>
+      </c>
+      <c r="I7">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="J7">
+        <v>0.107</v>
+      </c>
+      <c r="K7">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="L7">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.105</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1.0629999999999999</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1.0940000000000001</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1.159</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0.156</v>
+      </c>
+      <c r="J8" s="7">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0.107</v>
+      </c>
+      <c r="L8">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9.4E-2</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1.077</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0.106</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="L9">
+        <v>9.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.1</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1.073</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1.0509999999999999</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1.04</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0.317</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="L10">
+        <v>0.10100000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="B11">
+        <v>1.0860000000000001</v>
+      </c>
+      <c r="C11">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="D11">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="E11">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="F11">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="G11">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="H11">
+        <v>0.376</v>
+      </c>
+      <c r="I11">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="J11">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="K11">
+        <v>0.191</v>
+      </c>
+      <c r="L11">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="B12">
+        <v>1.0589999999999999</v>
+      </c>
+      <c r="C12">
+        <v>0.995</v>
+      </c>
+      <c r="D12">
+        <v>1.006</v>
+      </c>
+      <c r="E12">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="F12">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="G12">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="H12">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="I12">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="J12">
+        <v>0.184</v>
+      </c>
+      <c r="K12">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="L12">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="B13">
+        <v>1.04</v>
+      </c>
+      <c r="C13">
+        <v>0.996</v>
+      </c>
+      <c r="D13">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="F13">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="G13">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="H13">
+        <v>0.378</v>
+      </c>
+      <c r="I13">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="J13">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="K13">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="L13">
+        <v>7.8E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="B14">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="C14">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="D14">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="E14">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F14">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="G14">
+        <v>7.8E-2</v>
+      </c>
+      <c r="H14">
+        <v>0.08</v>
+      </c>
+      <c r="I14">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="J14">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="K14">
+        <v>7.8E-2</v>
+      </c>
+      <c r="L14">
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>AVERAGE(B8:B10)</f>
+        <v>1.0603333333333331</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:K16" si="0">AVERAGE(C8:C10)</f>
+        <v>0.97266666666666668</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1.0919999999999999</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0.67433333333333334</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0.8706666666666667</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0.315</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>0.11466666666666665</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1.0603333333333331</v>
+      </c>
+      <c r="C18" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>0.97266666666666668</v>
+      </c>
+      <c r="C19" s="1">
+        <f>B19/1.060333*100</f>
+        <v>91.73218853573988</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1.0919999999999999</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" ref="C20:C27" si="1">B20/1.060333*100</f>
+        <v>102.98651461380528</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>0.67433333333333334</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="1"/>
+        <v>63.596373340576342</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>0.8706666666666667</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="1"/>
+        <v>82.112569038845976</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>0.315</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="1"/>
+        <v>29.707648446289987</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="1"/>
+        <v>13.014779319327044</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="1"/>
+        <v>13.957879270002913</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="1"/>
+        <v>9.6196194968939004</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>0.11466666666666665</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="1"/>
+        <v>10.814212767750005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>